<commit_message>
tocas_fram fixing a few missing leading 0s, adding explicit Dispositions
</commit_message>
<xml_diff>
--- a/xlsx/lu_coho.xlsx
+++ b/xlsx/lu_coho.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/daniel_auerbach_dfw_wa_gov/Documents/code/framr/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1046" documentId="8_{21B4543F-78BB-4220-988B-83DC0936FF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D932AA05-54A7-490F-9E96-A5A96842DF63}"/>
+  <xr:revisionPtr revIDLastSave="1071" documentId="8_{21B4543F-78BB-4220-988B-83DC0936FF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1849C25B-8FEF-4DAE-8E41-C9AEF9966D2C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{DF93BC40-F587-4C27-AB72-1CFE9880D23F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="349">
   <si>
     <t>area_code</t>
   </si>
@@ -692,9 +692,6 @@
     <t>TEST</t>
   </si>
   <si>
-    <t>8A</t>
-  </si>
-  <si>
     <t>Ar8A NetNT</t>
   </si>
   <si>
@@ -704,12 +701,6 @@
     <t>Ar8D NetNT</t>
   </si>
   <si>
-    <t>8D</t>
-  </si>
-  <si>
-    <t>8d</t>
-  </si>
-  <si>
     <t>Ar8D NetTR</t>
   </si>
   <si>
@@ -923,9 +914,6 @@
     <t>Ar9ANetTR</t>
   </si>
   <si>
-    <t>!TEST</t>
-  </si>
-  <si>
     <t>12A</t>
   </si>
   <si>
@@ -1083,6 +1071,21 @@
   </si>
   <si>
     <t>09A</t>
+  </si>
+  <si>
+    <t>08A</t>
+  </si>
+  <si>
+    <t>08D</t>
+  </si>
+  <si>
+    <t>08d</t>
+  </si>
+  <si>
+    <t>C&amp;SF,COMM,ORGN,TEST,TKHM</t>
+  </si>
+  <si>
+    <t>COMM,TKHM</t>
   </si>
 </sst>
 </file>
@@ -2841,8 +2844,8 @@
   <dimension ref="A1:G265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D242" sqref="D242:D265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2861,7 +2864,7 @@
         <v>155</v>
       </c>
       <c r="C1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D1" t="s">
         <v>213</v>
@@ -2873,7 +2876,7 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2883,6 +2886,9 @@
       <c r="C2">
         <v>41</v>
       </c>
+      <c r="D2" t="s">
+        <v>347</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2890,7 +2896,7 @@
         <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2900,6 +2906,9 @@
       <c r="C3">
         <v>41</v>
       </c>
+      <c r="D3" t="s">
+        <v>347</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2907,7 +2916,7 @@
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2917,6 +2926,9 @@
       <c r="C4">
         <v>41</v>
       </c>
+      <c r="D4" t="s">
+        <v>347</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2924,7 +2936,7 @@
         <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2934,6 +2946,9 @@
       <c r="C5">
         <v>41</v>
       </c>
+      <c r="D5" t="s">
+        <v>347</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2950,6 +2965,9 @@
       </c>
       <c r="C6">
         <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>347</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
@@ -2968,6 +2986,9 @@
       <c r="C7">
         <v>41</v>
       </c>
+      <c r="D7" t="s">
+        <v>347</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2975,7 +2996,7 @@
         <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2985,14 +3006,17 @@
       <c r="C8">
         <v>41</v>
       </c>
+      <c r="D8" t="s">
+        <v>347</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F8">
         <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -3002,14 +3026,17 @@
       <c r="C9">
         <v>41</v>
       </c>
+      <c r="D9" t="s">
+        <v>347</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F9">
         <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -3019,6 +3046,9 @@
       <c r="C10">
         <v>41</v>
       </c>
+      <c r="D10" t="s">
+        <v>347</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>6</v>
       </c>
@@ -3026,7 +3056,7 @@
         <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -3036,14 +3066,17 @@
       <c r="C11">
         <v>41</v>
       </c>
+      <c r="D11" t="s">
+        <v>347</v>
+      </c>
       <c r="E11" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F11">
         <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -3053,14 +3086,17 @@
       <c r="C12">
         <v>41</v>
       </c>
+      <c r="D12" t="s">
+        <v>347</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F12">
         <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -3068,7 +3104,10 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D13" t="s">
+        <v>347</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>6</v>
@@ -3077,7 +3116,7 @@
         <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -3085,16 +3124,19 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D14" t="s">
+        <v>347</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F14">
         <v>43</v>
       </c>
       <c r="G14" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -3102,16 +3144,19 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D15" t="s">
+        <v>347</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F15">
         <v>43</v>
       </c>
       <c r="G15" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -3121,6 +3166,9 @@
       <c r="C16">
         <v>41</v>
       </c>
+      <c r="D16" t="s">
+        <v>347</v>
+      </c>
       <c r="E16" s="1" t="s">
         <v>66</v>
       </c>
@@ -3128,7 +3176,7 @@
         <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -3138,6 +3186,9 @@
       <c r="C17">
         <v>41</v>
       </c>
+      <c r="D17" t="s">
+        <v>347</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>67</v>
       </c>
@@ -3145,7 +3196,7 @@
         <v>44</v>
       </c>
       <c r="G17" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -3155,14 +3206,17 @@
       <c r="C18">
         <v>41</v>
       </c>
+      <c r="D18" t="s">
+        <v>347</v>
+      </c>
       <c r="E18" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F18">
         <v>44</v>
       </c>
       <c r="G18" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -3172,14 +3226,17 @@
       <c r="C19">
         <v>41</v>
       </c>
+      <c r="D19" t="s">
+        <v>347</v>
+      </c>
       <c r="E19" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F19">
         <v>44</v>
       </c>
       <c r="G19" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -3189,6 +3246,9 @@
       <c r="C20">
         <v>41</v>
       </c>
+      <c r="D20" t="s">
+        <v>347</v>
+      </c>
       <c r="E20" t="s">
         <v>142</v>
       </c>
@@ -3196,7 +3256,7 @@
         <v>44</v>
       </c>
       <c r="G20" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -3204,7 +3264,10 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D21" t="s">
+        <v>347</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>66</v>
@@ -3213,7 +3276,7 @@
         <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -3221,7 +3284,10 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D22" t="s">
+        <v>347</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>67</v>
@@ -3230,7 +3296,7 @@
         <v>44</v>
       </c>
       <c r="G22" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -3238,16 +3304,19 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D23" t="s">
+        <v>347</v>
       </c>
       <c r="E23" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F23">
         <v>44</v>
       </c>
       <c r="G23" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -3255,16 +3324,19 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D24" t="s">
+        <v>347</v>
       </c>
       <c r="E24" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F24">
         <v>44</v>
       </c>
       <c r="G24" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -3272,7 +3344,10 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D25" t="s">
+        <v>347</v>
       </c>
       <c r="E25" t="s">
         <v>142</v>
@@ -3281,7 +3356,7 @@
         <v>44</v>
       </c>
       <c r="G25" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -3289,10 +3364,13 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D26" t="s">
+        <v>347</v>
       </c>
       <c r="E26" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F26">
         <v>47</v>
@@ -3306,10 +3384,13 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D27" t="s">
+        <v>347</v>
       </c>
       <c r="E27" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F27">
         <v>47</v>
@@ -3323,10 +3404,13 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D28" t="s">
+        <v>347</v>
       </c>
       <c r="E28" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F28">
         <v>47</v>
@@ -3340,10 +3424,13 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D29" t="s">
+        <v>347</v>
       </c>
       <c r="E29" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F29">
         <v>47</v>
@@ -3357,7 +3444,10 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D30" t="s">
+        <v>347</v>
       </c>
       <c r="E30" t="s">
         <v>143</v>
@@ -3374,7 +3464,10 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D31" t="s">
+        <v>347</v>
       </c>
       <c r="E31" t="s">
         <v>144</v>
@@ -3391,7 +3484,10 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D32" t="s">
+        <v>347</v>
       </c>
       <c r="E32" t="s">
         <v>145</v>
@@ -3408,7 +3504,10 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D33" t="s">
+        <v>347</v>
       </c>
       <c r="E33" t="s">
         <v>146</v>
@@ -3425,7 +3524,10 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D34" t="s">
+        <v>347</v>
       </c>
       <c r="E34" t="s">
         <v>147</v>
@@ -3442,10 +3544,13 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D35" t="s">
+        <v>347</v>
       </c>
       <c r="E35" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F35">
         <v>50</v>
@@ -3459,10 +3564,13 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D36" t="s">
+        <v>347</v>
       </c>
       <c r="E36" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F36">
         <v>50</v>
@@ -3476,10 +3584,13 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D37" t="s">
+        <v>347</v>
       </c>
       <c r="E37" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F37">
         <v>50</v>
@@ -3493,7 +3604,10 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D38" t="s">
+        <v>347</v>
       </c>
       <c r="E38" t="s">
         <v>148</v>
@@ -3513,10 +3627,13 @@
         <v>156</v>
       </c>
       <c r="C39" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D39" t="s">
+        <v>347</v>
       </c>
       <c r="E39" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F39">
         <v>52</v>
@@ -3533,10 +3650,13 @@
         <v>156</v>
       </c>
       <c r="C40" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D40" t="s">
+        <v>347</v>
       </c>
       <c r="E40" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F40">
         <v>52</v>
@@ -3553,7 +3673,10 @@
         <v>156</v>
       </c>
       <c r="C41" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D41" t="s">
+        <v>347</v>
       </c>
       <c r="E41" t="s">
         <v>148</v>
@@ -3573,7 +3696,10 @@
         <v>156</v>
       </c>
       <c r="C42" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D42" t="s">
+        <v>347</v>
       </c>
       <c r="E42" t="s">
         <v>157</v>
@@ -3590,10 +3716,13 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D43" t="s">
+        <v>347</v>
       </c>
       <c r="E43" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F43">
         <v>55</v>
@@ -3607,7 +3736,10 @@
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D44" t="s">
+        <v>347</v>
       </c>
       <c r="E44" t="s">
         <v>160</v>
@@ -3627,7 +3759,10 @@
         <v>161</v>
       </c>
       <c r="C45" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D45" t="s">
+        <v>347</v>
       </c>
       <c r="E45" t="s">
         <v>157</v>
@@ -3644,7 +3779,10 @@
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D46" t="s">
+        <v>347</v>
       </c>
       <c r="E46" t="s">
         <v>163</v>
@@ -3661,7 +3799,10 @@
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D47" t="s">
+        <v>347</v>
       </c>
       <c r="E47" t="s">
         <v>164</v>
@@ -3678,7 +3819,10 @@
         <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D48" t="s">
+        <v>347</v>
       </c>
       <c r="E48" t="s">
         <v>165</v>
@@ -3695,7 +3839,10 @@
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D49" t="s">
+        <v>347</v>
       </c>
       <c r="E49" t="s">
         <v>163</v>
@@ -3712,7 +3859,10 @@
         <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D50" t="s">
+        <v>347</v>
       </c>
       <c r="E50" t="s">
         <v>164</v>
@@ -3729,7 +3879,10 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D51" t="s">
+        <v>347</v>
       </c>
       <c r="E51" t="s">
         <v>165</v>
@@ -3746,7 +3899,10 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D52" t="s">
+        <v>347</v>
       </c>
       <c r="E52" t="s">
         <v>167</v>
@@ -3763,7 +3919,10 @@
         <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D53" t="s">
+        <v>347</v>
       </c>
       <c r="E53" t="s">
         <v>168</v>
@@ -3780,7 +3939,10 @@
         <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D54" t="s">
+        <v>347</v>
       </c>
       <c r="E54" t="s">
         <v>167</v>
@@ -3797,7 +3959,10 @@
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D55" t="s">
+        <v>347</v>
       </c>
       <c r="E55" t="s">
         <v>168</v>
@@ -3814,7 +3979,10 @@
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D56" t="s">
+        <v>347</v>
       </c>
       <c r="E56" t="s">
         <v>172</v>
@@ -3831,7 +3999,10 @@
         <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D57" t="s">
+        <v>347</v>
       </c>
       <c r="E57" t="s">
         <v>173</v>
@@ -3848,7 +4019,10 @@
         <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D58" t="s">
+        <v>347</v>
       </c>
       <c r="E58" t="s">
         <v>174</v>
@@ -3865,7 +4039,10 @@
         <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D59" t="s">
+        <v>347</v>
       </c>
       <c r="E59" t="s">
         <v>175</v>
@@ -3882,7 +4059,10 @@
         <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D60" t="s">
+        <v>347</v>
       </c>
       <c r="E60" t="s">
         <v>176</v>
@@ -3899,7 +4079,7 @@
         <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D61" t="s">
         <v>178</v>
@@ -3919,7 +4099,7 @@
         <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D62" t="s">
         <v>178</v>
@@ -3939,7 +4119,7 @@
         <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D63" t="s">
         <v>178</v>
@@ -3959,7 +4139,7 @@
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D64" t="s">
         <v>178</v>
@@ -3979,7 +4159,7 @@
         <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D65" t="s">
         <v>178</v>
@@ -3999,7 +4179,10 @@
         <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D66" t="s">
+        <v>347</v>
       </c>
       <c r="E66" t="s">
         <v>179</v>
@@ -4016,7 +4199,10 @@
         <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D67" t="s">
+        <v>347</v>
       </c>
       <c r="E67" t="s">
         <v>179</v>
@@ -4033,7 +4219,10 @@
         <v>2</v>
       </c>
       <c r="C68" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D68" t="s">
+        <v>347</v>
       </c>
       <c r="E68" t="s">
         <v>179</v>
@@ -4050,7 +4239,10 @@
         <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D69" t="s">
+        <v>347</v>
       </c>
       <c r="E69" t="s">
         <v>182</v>
@@ -4067,7 +4259,10 @@
         <v>2</v>
       </c>
       <c r="C70" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D70" t="s">
+        <v>347</v>
       </c>
       <c r="E70" t="s">
         <v>183</v>
@@ -4084,7 +4279,10 @@
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D71" t="s">
+        <v>347</v>
       </c>
       <c r="E71" t="s">
         <v>184</v>
@@ -4101,7 +4299,10 @@
         <v>2</v>
       </c>
       <c r="C72" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D72" t="s">
+        <v>347</v>
       </c>
       <c r="E72" t="s">
         <v>182</v>
@@ -4118,7 +4319,10 @@
         <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D73" t="s">
+        <v>347</v>
       </c>
       <c r="E73" t="s">
         <v>183</v>
@@ -4135,7 +4339,10 @@
         <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D74" t="s">
+        <v>347</v>
       </c>
       <c r="E74" t="s">
         <v>184</v>
@@ -4152,16 +4359,19 @@
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D75" t="s">
+        <v>347</v>
       </c>
       <c r="E75" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F75">
         <v>80</v>
       </c>
       <c r="G75" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -4169,7 +4379,10 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D76" t="s">
+        <v>347</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>66</v>
@@ -4178,7 +4391,7 @@
         <v>80</v>
       </c>
       <c r="G76" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -4186,7 +4399,10 @@
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D77" t="s">
+        <v>347</v>
       </c>
       <c r="E77" t="s">
         <v>142</v>
@@ -4195,7 +4411,7 @@
         <v>80</v>
       </c>
       <c r="G77" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -4203,16 +4419,19 @@
         <v>2</v>
       </c>
       <c r="C78" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D78" t="s">
+        <v>347</v>
       </c>
       <c r="E78" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F78">
         <v>81</v>
       </c>
       <c r="G78" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -4220,7 +4439,10 @@
         <v>2</v>
       </c>
       <c r="C79" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D79" t="s">
+        <v>347</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>66</v>
@@ -4229,7 +4451,7 @@
         <v>81</v>
       </c>
       <c r="G79" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -4237,7 +4459,10 @@
         <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D80" t="s">
+        <v>347</v>
       </c>
       <c r="E80" t="s">
         <v>142</v>
@@ -4246,7 +4471,7 @@
         <v>81</v>
       </c>
       <c r="G80" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -4254,16 +4479,19 @@
         <v>1</v>
       </c>
       <c r="C81" t="s">
+        <v>312</v>
+      </c>
+      <c r="D81" t="s">
+        <v>347</v>
+      </c>
+      <c r="E81" t="s">
         <v>316</v>
-      </c>
-      <c r="E81" t="s">
-        <v>320</v>
       </c>
       <c r="F81">
         <v>82</v>
       </c>
       <c r="G81" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -4271,16 +4499,19 @@
         <v>2</v>
       </c>
       <c r="C82" t="s">
+        <v>312</v>
+      </c>
+      <c r="D82" t="s">
+        <v>347</v>
+      </c>
+      <c r="E82" t="s">
         <v>316</v>
-      </c>
-      <c r="E82" t="s">
-        <v>320</v>
       </c>
       <c r="F82">
         <v>83</v>
       </c>
       <c r="G82" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -4288,7 +4519,10 @@
         <v>2</v>
       </c>
       <c r="C83" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D83" t="s">
+        <v>347</v>
       </c>
       <c r="E83" t="s">
         <v>186</v>
@@ -4297,7 +4531,7 @@
         <v>83</v>
       </c>
       <c r="G83" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -4305,16 +4539,19 @@
         <v>2</v>
       </c>
       <c r="C84" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D84" t="s">
+        <v>347</v>
       </c>
       <c r="E84" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F84">
         <v>83</v>
       </c>
       <c r="G84" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -4322,7 +4559,10 @@
         <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D85" t="s">
+        <v>347</v>
       </c>
       <c r="E85" t="s">
         <v>186</v>
@@ -4331,7 +4571,7 @@
         <v>83</v>
       </c>
       <c r="G85" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -4339,7 +4579,10 @@
         <v>2</v>
       </c>
       <c r="C86" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D86" t="s">
+        <v>347</v>
       </c>
       <c r="E86" t="s">
         <v>187</v>
@@ -4356,7 +4599,10 @@
         <v>2</v>
       </c>
       <c r="C87" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D87" t="s">
+        <v>347</v>
       </c>
       <c r="E87" t="s">
         <v>187</v>
@@ -4373,7 +4619,10 @@
         <v>2</v>
       </c>
       <c r="C88" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D88" t="s">
+        <v>347</v>
       </c>
       <c r="E88" t="s">
         <v>189</v>
@@ -4390,7 +4639,10 @@
         <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D89" t="s">
+        <v>347</v>
       </c>
       <c r="E89" t="s">
         <v>190</v>
@@ -4407,7 +4659,10 @@
         <v>2</v>
       </c>
       <c r="C90" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D90" t="s">
+        <v>347</v>
       </c>
       <c r="E90" t="s">
         <v>193</v>
@@ -4424,7 +4679,10 @@
         <v>2</v>
       </c>
       <c r="C91" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D91" t="s">
+        <v>347</v>
       </c>
       <c r="E91" t="s">
         <v>194</v>
@@ -4441,7 +4699,10 @@
         <v>2</v>
       </c>
       <c r="C92" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D92" t="s">
+        <v>347</v>
       </c>
       <c r="E92" t="s">
         <v>195</v>
@@ -4458,7 +4719,10 @@
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D93" t="s">
+        <v>347</v>
       </c>
       <c r="E93" t="s">
         <v>192</v>
@@ -4475,7 +4739,10 @@
         <v>2</v>
       </c>
       <c r="C94" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D94" t="s">
+        <v>347</v>
       </c>
       <c r="E94" t="s">
         <v>191</v>
@@ -4492,7 +4759,10 @@
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D95" t="s">
+        <v>347</v>
       </c>
       <c r="E95" t="s">
         <v>196</v>
@@ -4509,7 +4779,10 @@
         <v>2</v>
       </c>
       <c r="C96" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D96" t="s">
+        <v>347</v>
       </c>
       <c r="E96" t="s">
         <v>197</v>
@@ -4526,7 +4799,10 @@
         <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D97" t="s">
+        <v>347</v>
       </c>
       <c r="E97" t="s">
         <v>189</v>
@@ -4543,7 +4819,10 @@
         <v>2</v>
       </c>
       <c r="C98" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D98" t="s">
+        <v>347</v>
       </c>
       <c r="E98" t="s">
         <v>190</v>
@@ -4560,7 +4839,10 @@
         <v>2</v>
       </c>
       <c r="C99" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D99" t="s">
+        <v>347</v>
       </c>
       <c r="E99" t="s">
         <v>193</v>
@@ -4577,7 +4859,10 @@
         <v>2</v>
       </c>
       <c r="C100" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D100" t="s">
+        <v>347</v>
       </c>
       <c r="E100" t="s">
         <v>194</v>
@@ -4594,7 +4879,10 @@
         <v>2</v>
       </c>
       <c r="C101" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D101" t="s">
+        <v>347</v>
       </c>
       <c r="E101" t="s">
         <v>195</v>
@@ -4611,7 +4899,10 @@
         <v>2</v>
       </c>
       <c r="C102" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D102" t="s">
+        <v>347</v>
       </c>
       <c r="E102" t="s">
         <v>192</v>
@@ -4628,7 +4919,10 @@
         <v>2</v>
       </c>
       <c r="C103" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D103" t="s">
+        <v>347</v>
       </c>
       <c r="E103" t="s">
         <v>191</v>
@@ -4645,7 +4939,10 @@
         <v>2</v>
       </c>
       <c r="C104" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D104" t="s">
+        <v>347</v>
       </c>
       <c r="E104" t="s">
         <v>196</v>
@@ -4662,7 +4959,10 @@
         <v>2</v>
       </c>
       <c r="C105" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D105" t="s">
+        <v>347</v>
       </c>
       <c r="E105" t="s">
         <v>197</v>
@@ -4679,7 +4979,10 @@
         <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D106" t="s">
+        <v>347</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>67</v>
@@ -4688,7 +4991,7 @@
         <v>87</v>
       </c>
       <c r="G106" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
@@ -4696,16 +4999,19 @@
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D107" t="s">
+        <v>347</v>
       </c>
       <c r="E107" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F107">
         <v>87</v>
       </c>
       <c r="G107" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
@@ -4713,16 +5019,19 @@
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D108" t="s">
+        <v>347</v>
       </c>
       <c r="E108" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F108">
         <v>87</v>
       </c>
       <c r="G108" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
@@ -4730,7 +5039,10 @@
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D109" t="s">
+        <v>347</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>68</v>
@@ -4739,7 +5051,7 @@
         <v>87</v>
       </c>
       <c r="G109" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
@@ -4747,16 +5059,19 @@
         <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D110" t="s">
+        <v>347</v>
       </c>
       <c r="E110" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F110">
         <v>87</v>
       </c>
       <c r="G110" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
@@ -4764,16 +5079,19 @@
         <v>1</v>
       </c>
       <c r="C111" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D111" t="s">
+        <v>347</v>
       </c>
       <c r="E111" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F111">
         <v>87</v>
       </c>
       <c r="G111" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -4781,7 +5099,10 @@
         <v>2</v>
       </c>
       <c r="C112" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D112" t="s">
+        <v>347</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>67</v>
@@ -4790,7 +5111,7 @@
         <v>87</v>
       </c>
       <c r="G112" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
@@ -4798,16 +5119,19 @@
         <v>2</v>
       </c>
       <c r="C113" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D113" t="s">
+        <v>347</v>
       </c>
       <c r="E113" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F113">
         <v>87</v>
       </c>
       <c r="G113" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -4815,16 +5139,19 @@
         <v>2</v>
       </c>
       <c r="C114" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D114" t="s">
+        <v>347</v>
       </c>
       <c r="E114" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F114">
         <v>87</v>
       </c>
       <c r="G114" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
@@ -4832,7 +5159,10 @@
         <v>2</v>
       </c>
       <c r="C115" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D115" t="s">
+        <v>347</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>68</v>
@@ -4841,7 +5171,7 @@
         <v>87</v>
       </c>
       <c r="G115" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
@@ -4849,16 +5179,19 @@
         <v>2</v>
       </c>
       <c r="C116" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D116" t="s">
+        <v>347</v>
       </c>
       <c r="E116" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F116">
         <v>87</v>
       </c>
       <c r="G116" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
@@ -4866,16 +5199,19 @@
         <v>2</v>
       </c>
       <c r="C117" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D117" t="s">
+        <v>347</v>
       </c>
       <c r="E117" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F117">
         <v>87</v>
       </c>
       <c r="G117" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -4883,16 +5219,19 @@
         <v>1</v>
       </c>
       <c r="C118" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D118" t="s">
+        <v>347</v>
       </c>
       <c r="E118" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F118">
         <v>96</v>
       </c>
       <c r="G118" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
@@ -4900,16 +5239,19 @@
         <v>1</v>
       </c>
       <c r="C119" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D119" t="s">
+        <v>347</v>
       </c>
       <c r="E119" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F119">
         <v>96</v>
       </c>
       <c r="G119" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
@@ -4917,16 +5259,19 @@
         <v>1</v>
       </c>
       <c r="C120" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D120" t="s">
+        <v>347</v>
       </c>
       <c r="E120" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F120">
         <v>96</v>
       </c>
       <c r="G120" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
@@ -4934,16 +5279,19 @@
         <v>2</v>
       </c>
       <c r="C121" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D121" t="s">
+        <v>347</v>
       </c>
       <c r="E121" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F121">
         <v>97</v>
       </c>
       <c r="G121" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
@@ -4951,16 +5299,19 @@
         <v>2</v>
       </c>
       <c r="C122" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D122" t="s">
+        <v>347</v>
       </c>
       <c r="E122" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F122">
         <v>97</v>
       </c>
       <c r="G122" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
@@ -4968,16 +5319,19 @@
         <v>2</v>
       </c>
       <c r="C123" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D123" t="s">
+        <v>347</v>
       </c>
       <c r="E123" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F123">
         <v>97</v>
       </c>
       <c r="G123" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
@@ -4985,7 +5339,10 @@
         <v>2</v>
       </c>
       <c r="C124" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D124" t="s">
+        <v>347</v>
       </c>
       <c r="E124" t="s">
         <v>200</v>
@@ -5002,7 +5359,10 @@
         <v>2</v>
       </c>
       <c r="C125" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D125" t="s">
+        <v>347</v>
       </c>
       <c r="E125" t="s">
         <v>201</v>
@@ -5019,10 +5379,13 @@
         <v>1</v>
       </c>
       <c r="C126" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D126" t="s">
+        <v>347</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F126">
         <v>101</v>
@@ -5036,10 +5399,13 @@
         <v>2</v>
       </c>
       <c r="C127" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D127" t="s">
+        <v>347</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F127">
         <v>102</v>
@@ -5053,7 +5419,10 @@
         <v>2</v>
       </c>
       <c r="C128" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D128" t="s">
+        <v>347</v>
       </c>
       <c r="E128" t="s">
         <v>204</v>
@@ -5070,7 +5439,10 @@
         <v>2</v>
       </c>
       <c r="C129" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D129" t="s">
+        <v>347</v>
       </c>
       <c r="E129" t="s">
         <v>205</v>
@@ -5087,7 +5459,10 @@
         <v>2</v>
       </c>
       <c r="C130" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D130" t="s">
+        <v>347</v>
       </c>
       <c r="E130" t="s">
         <v>206</v>
@@ -5104,7 +5479,10 @@
         <v>2</v>
       </c>
       <c r="C131" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D131" t="s">
+        <v>347</v>
       </c>
       <c r="E131" t="s">
         <v>207</v>
@@ -5121,7 +5499,10 @@
         <v>2</v>
       </c>
       <c r="C132" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D132" t="s">
+        <v>347</v>
       </c>
       <c r="E132" t="s">
         <v>208</v>
@@ -5138,7 +5519,10 @@
         <v>2</v>
       </c>
       <c r="C133" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D133" t="s">
+        <v>347</v>
       </c>
       <c r="E133" t="s">
         <v>209</v>
@@ -5155,7 +5539,10 @@
         <v>2</v>
       </c>
       <c r="C134" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D134" t="s">
+        <v>347</v>
       </c>
       <c r="E134" t="s">
         <v>210</v>
@@ -5172,7 +5559,10 @@
         <v>2</v>
       </c>
       <c r="C135" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D135" t="s">
+        <v>347</v>
       </c>
       <c r="E135" t="s">
         <v>211</v>
@@ -5189,7 +5579,7 @@
         <v>2</v>
       </c>
       <c r="C136" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D136" t="s">
         <v>215</v>
@@ -5209,7 +5599,7 @@
         <v>2</v>
       </c>
       <c r="C137" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D137" t="s">
         <v>215</v>
@@ -5229,7 +5619,7 @@
         <v>2</v>
       </c>
       <c r="C138" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D138" t="s">
         <v>215</v>
@@ -5249,7 +5639,7 @@
         <v>2</v>
       </c>
       <c r="C139" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D139" t="s">
         <v>215</v>
@@ -5269,7 +5659,7 @@
         <v>2</v>
       </c>
       <c r="C140" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D140" t="s">
         <v>215</v>
@@ -5289,7 +5679,7 @@
         <v>2</v>
       </c>
       <c r="C141" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D141" t="s">
         <v>215</v>
@@ -5309,7 +5699,7 @@
         <v>2</v>
       </c>
       <c r="C142" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D142" t="s">
         <v>215</v>
@@ -5329,7 +5719,7 @@
         <v>2</v>
       </c>
       <c r="C143" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D143" t="s">
         <v>215</v>
@@ -5349,7 +5739,7 @@
         <v>2</v>
       </c>
       <c r="C144" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D144" t="s">
         <v>216</v>
@@ -5369,7 +5759,7 @@
         <v>2</v>
       </c>
       <c r="C145" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D145" t="s">
         <v>216</v>
@@ -5389,7 +5779,7 @@
         <v>2</v>
       </c>
       <c r="C146" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D146" t="s">
         <v>216</v>
@@ -5409,7 +5799,7 @@
         <v>2</v>
       </c>
       <c r="C147" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D147" t="s">
         <v>216</v>
@@ -5429,7 +5819,7 @@
         <v>2</v>
       </c>
       <c r="C148" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D148" t="s">
         <v>216</v>
@@ -5449,7 +5839,7 @@
         <v>2</v>
       </c>
       <c r="C149" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D149" t="s">
         <v>216</v>
@@ -5469,7 +5859,7 @@
         <v>2</v>
       </c>
       <c r="C150" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D150" t="s">
         <v>216</v>
@@ -5489,7 +5879,7 @@
         <v>2</v>
       </c>
       <c r="C151" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D151" t="s">
         <v>216</v>
@@ -5509,16 +5899,19 @@
         <v>1</v>
       </c>
       <c r="C152" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D152" t="s">
+        <v>347</v>
       </c>
       <c r="E152" t="s">
-        <v>217</v>
+        <v>344</v>
       </c>
       <c r="F152">
         <v>109</v>
       </c>
       <c r="G152" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
@@ -5526,16 +5919,19 @@
         <v>2</v>
       </c>
       <c r="C153" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D153" t="s">
+        <v>347</v>
       </c>
       <c r="E153" t="s">
-        <v>217</v>
+        <v>344</v>
       </c>
       <c r="F153">
         <v>110</v>
       </c>
       <c r="G153" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -5543,16 +5939,19 @@
         <v>2</v>
       </c>
       <c r="C154" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D154" t="s">
+        <v>347</v>
       </c>
       <c r="E154" t="s">
-        <v>217</v>
+        <v>344</v>
       </c>
       <c r="F154">
         <v>110</v>
       </c>
       <c r="G154" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
@@ -5560,16 +5959,19 @@
         <v>1</v>
       </c>
       <c r="C155" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D155" t="s">
+        <v>347</v>
       </c>
       <c r="E155" t="s">
-        <v>221</v>
+        <v>345</v>
       </c>
       <c r="F155">
         <v>111</v>
       </c>
       <c r="G155" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
@@ -5577,16 +5979,19 @@
         <v>1</v>
       </c>
       <c r="C156" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D156" t="s">
+        <v>347</v>
       </c>
       <c r="E156" t="s">
-        <v>222</v>
+        <v>346</v>
       </c>
       <c r="F156">
         <v>111</v>
       </c>
       <c r="G156" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
@@ -5594,16 +5999,19 @@
         <v>2</v>
       </c>
       <c r="C157" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D157" t="s">
+        <v>347</v>
       </c>
       <c r="E157" t="s">
-        <v>221</v>
+        <v>345</v>
       </c>
       <c r="F157">
         <v>112</v>
       </c>
       <c r="G157" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
@@ -5611,16 +6019,19 @@
         <v>2</v>
       </c>
       <c r="C158" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D158" t="s">
+        <v>347</v>
       </c>
       <c r="E158" t="s">
-        <v>222</v>
+        <v>346</v>
       </c>
       <c r="F158">
         <v>112</v>
       </c>
       <c r="G158" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
@@ -5628,16 +6039,19 @@
         <v>2</v>
       </c>
       <c r="C159" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D159" t="s">
+        <v>347</v>
       </c>
       <c r="E159" t="s">
-        <v>221</v>
+        <v>345</v>
       </c>
       <c r="F159">
         <v>112</v>
       </c>
       <c r="G159" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
@@ -5645,16 +6059,19 @@
         <v>2</v>
       </c>
       <c r="C160" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D160" t="s">
+        <v>347</v>
       </c>
       <c r="E160" t="s">
-        <v>222</v>
+        <v>346</v>
       </c>
       <c r="F160">
         <v>112</v>
       </c>
       <c r="G160" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
@@ -5662,16 +6079,19 @@
         <v>2</v>
       </c>
       <c r="C161" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D161" t="s">
+        <v>347</v>
       </c>
       <c r="E161" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F161">
         <v>113</v>
       </c>
       <c r="G161" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
@@ -5679,16 +6099,19 @@
         <v>2</v>
       </c>
       <c r="C162" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D162" t="s">
+        <v>347</v>
       </c>
       <c r="E162" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F162">
         <v>114</v>
       </c>
       <c r="G162" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
@@ -5696,16 +6119,19 @@
         <v>2</v>
       </c>
       <c r="C163" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D163" t="s">
+        <v>347</v>
       </c>
       <c r="E163" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F163">
         <v>114</v>
       </c>
       <c r="G163" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
@@ -5713,16 +6139,19 @@
         <v>2</v>
       </c>
       <c r="C164" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D164" t="s">
+        <v>347</v>
       </c>
       <c r="E164" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F164">
         <v>114</v>
       </c>
       <c r="G164" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
@@ -5730,16 +6159,19 @@
         <v>2</v>
       </c>
       <c r="C165" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D165" t="s">
+        <v>347</v>
       </c>
       <c r="E165" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F165">
         <v>114</v>
       </c>
       <c r="G165" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
@@ -5747,16 +6179,19 @@
         <v>2</v>
       </c>
       <c r="C166" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D166" t="s">
+        <v>347</v>
       </c>
       <c r="E166" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F166">
         <v>114</v>
       </c>
       <c r="G166" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
@@ -5764,7 +6199,10 @@
         <v>1</v>
       </c>
       <c r="C167" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D167" t="s">
+        <v>347</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>99</v>
@@ -5773,7 +6211,7 @@
         <v>119</v>
       </c>
       <c r="G167" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
@@ -5781,7 +6219,10 @@
         <v>2</v>
       </c>
       <c r="C168" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D168" t="s">
+        <v>347</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>99</v>
@@ -5790,7 +6231,7 @@
         <v>120</v>
       </c>
       <c r="G168" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
@@ -5798,16 +6239,19 @@
         <v>2</v>
       </c>
       <c r="C169" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D169" t="s">
+        <v>347</v>
       </c>
       <c r="E169" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F169">
         <v>120</v>
       </c>
       <c r="G169" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
@@ -5815,16 +6259,19 @@
         <v>1</v>
       </c>
       <c r="C170" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D170" t="s">
+        <v>347</v>
       </c>
       <c r="E170" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F170">
         <v>121</v>
       </c>
       <c r="G170" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
@@ -5832,16 +6279,19 @@
         <v>1</v>
       </c>
       <c r="C171" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D171" t="s">
+        <v>347</v>
       </c>
       <c r="E171" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F171">
         <v>121</v>
       </c>
       <c r="G171" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
@@ -5849,16 +6299,19 @@
         <v>2</v>
       </c>
       <c r="C172" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D172" t="s">
+        <v>347</v>
       </c>
       <c r="E172" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F172">
         <v>122</v>
       </c>
       <c r="G172" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
@@ -5866,16 +6319,19 @@
         <v>2</v>
       </c>
       <c r="C173" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D173" t="s">
+        <v>347</v>
       </c>
       <c r="E173" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F173">
         <v>122</v>
       </c>
       <c r="G173" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
@@ -5883,16 +6339,19 @@
         <v>1</v>
       </c>
       <c r="C174" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D174" t="s">
+        <v>347</v>
       </c>
       <c r="E174" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F174">
         <v>123</v>
       </c>
       <c r="G174" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
@@ -5900,16 +6359,19 @@
         <v>2</v>
       </c>
       <c r="C175" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D175" t="s">
+        <v>347</v>
       </c>
       <c r="E175" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F175">
         <v>124</v>
       </c>
       <c r="G175" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
@@ -5917,16 +6379,19 @@
         <v>2</v>
       </c>
       <c r="C176" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D176" t="s">
+        <v>347</v>
       </c>
       <c r="E176" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F176">
         <v>125</v>
       </c>
       <c r="G176" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
@@ -5934,16 +6399,19 @@
         <v>2</v>
       </c>
       <c r="C177" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D177" t="s">
+        <v>347</v>
       </c>
       <c r="E177" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F177">
         <v>125</v>
       </c>
       <c r="G177" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
@@ -5951,16 +6419,19 @@
         <v>2</v>
       </c>
       <c r="C178" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D178" t="s">
+        <v>347</v>
       </c>
       <c r="E178" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F178">
         <v>125</v>
       </c>
       <c r="G178" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.3">
@@ -5968,16 +6439,19 @@
         <v>2</v>
       </c>
       <c r="C179" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D179" t="s">
+        <v>347</v>
       </c>
       <c r="E179" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F179">
         <v>125</v>
       </c>
       <c r="G179" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
@@ -5985,16 +6459,19 @@
         <v>2</v>
       </c>
       <c r="C180" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D180" t="s">
+        <v>347</v>
       </c>
       <c r="E180" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F180">
         <v>125</v>
       </c>
       <c r="G180" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
@@ -6002,16 +6479,19 @@
         <v>2</v>
       </c>
       <c r="C181" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D181" t="s">
+        <v>347</v>
       </c>
       <c r="E181" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F181">
         <v>125</v>
       </c>
       <c r="G181" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
@@ -6019,16 +6499,19 @@
         <v>2</v>
       </c>
       <c r="C182" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D182" t="s">
+        <v>347</v>
       </c>
       <c r="E182" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F182">
         <v>125</v>
       </c>
       <c r="G182" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.3">
@@ -6036,16 +6519,19 @@
         <v>2</v>
       </c>
       <c r="C183" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D183" t="s">
+        <v>347</v>
       </c>
       <c r="E183" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F183">
         <v>126</v>
       </c>
       <c r="G183" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">
@@ -6053,16 +6539,19 @@
         <v>2</v>
       </c>
       <c r="C184" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D184" t="s">
+        <v>347</v>
       </c>
       <c r="E184" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F184">
         <v>126</v>
       </c>
       <c r="G184" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.3">
@@ -6070,7 +6559,10 @@
         <v>1</v>
       </c>
       <c r="C185" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D185" t="s">
+        <v>347</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>105</v>
@@ -6079,7 +6571,7 @@
         <v>130</v>
       </c>
       <c r="G185" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.3">
@@ -6087,7 +6579,10 @@
         <v>2</v>
       </c>
       <c r="C186" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D186" t="s">
+        <v>347</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>105</v>
@@ -6096,7 +6591,7 @@
         <v>131</v>
       </c>
       <c r="G186" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
@@ -6104,16 +6599,19 @@
         <v>1</v>
       </c>
       <c r="C187" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D187" t="s">
+        <v>347</v>
       </c>
       <c r="E187" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F187">
         <v>132</v>
       </c>
       <c r="G187" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.3">
@@ -6121,16 +6619,19 @@
         <v>2</v>
       </c>
       <c r="C188" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D188" t="s">
+        <v>347</v>
       </c>
       <c r="E188" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F188">
         <v>133</v>
       </c>
       <c r="G188" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
@@ -6138,16 +6639,19 @@
         <v>2</v>
       </c>
       <c r="C189" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D189" t="s">
+        <v>347</v>
       </c>
       <c r="E189" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F189">
         <v>134</v>
       </c>
       <c r="G189" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
@@ -6155,16 +6659,19 @@
         <v>2</v>
       </c>
       <c r="C190" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D190" t="s">
+        <v>347</v>
       </c>
       <c r="E190" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F190">
         <v>134</v>
       </c>
       <c r="G190" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
@@ -6172,16 +6679,19 @@
         <v>2</v>
       </c>
       <c r="C191" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D191" t="s">
+        <v>347</v>
       </c>
       <c r="E191" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F191">
         <v>134</v>
       </c>
       <c r="G191" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.3">
@@ -6189,16 +6699,19 @@
         <v>2</v>
       </c>
       <c r="C192" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D192" t="s">
+        <v>347</v>
       </c>
       <c r="E192" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F192">
         <v>134</v>
       </c>
       <c r="G192" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
@@ -6206,16 +6719,19 @@
         <v>2</v>
       </c>
       <c r="C193" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D193" t="s">
+        <v>347</v>
       </c>
       <c r="E193" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F193">
         <v>134</v>
       </c>
       <c r="G193" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.3">
@@ -6223,16 +6739,19 @@
         <v>2</v>
       </c>
       <c r="C194" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D194" t="s">
+        <v>347</v>
       </c>
       <c r="E194" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F194">
         <v>134</v>
       </c>
       <c r="G194" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
@@ -6240,16 +6759,19 @@
         <v>5</v>
       </c>
       <c r="C195" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D195" t="s">
+        <v>347</v>
       </c>
       <c r="E195" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F195">
         <v>134</v>
       </c>
       <c r="G195" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.3">
@@ -6257,16 +6779,19 @@
         <v>5</v>
       </c>
       <c r="C196" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D196" t="s">
+        <v>347</v>
       </c>
       <c r="E196" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F196">
         <v>134</v>
       </c>
       <c r="G196" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.3">
@@ -6274,16 +6799,19 @@
         <v>5</v>
       </c>
       <c r="C197" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D197" t="s">
+        <v>347</v>
       </c>
       <c r="E197" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F197">
         <v>134</v>
       </c>
       <c r="G197" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.3">
@@ -6291,16 +6819,19 @@
         <v>5</v>
       </c>
       <c r="C198" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D198" t="s">
+        <v>347</v>
       </c>
       <c r="E198" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F198">
         <v>134</v>
       </c>
       <c r="G198" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
@@ -6308,16 +6839,19 @@
         <v>5</v>
       </c>
       <c r="C199" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D199" t="s">
+        <v>347</v>
       </c>
       <c r="E199" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F199">
         <v>134</v>
       </c>
       <c r="G199" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
@@ -6325,16 +6859,19 @@
         <v>5</v>
       </c>
       <c r="C200" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D200" t="s">
+        <v>347</v>
       </c>
       <c r="E200" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F200">
         <v>134</v>
       </c>
       <c r="G200" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.3">
@@ -6342,7 +6879,10 @@
         <v>1</v>
       </c>
       <c r="C201" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D201" t="s">
+        <v>347</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>110</v>
@@ -6351,7 +6891,7 @@
         <v>137</v>
       </c>
       <c r="G201" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.3">
@@ -6359,16 +6899,19 @@
         <v>1</v>
       </c>
       <c r="C202" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D202" t="s">
+        <v>347</v>
       </c>
       <c r="E202" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F202">
         <v>137</v>
       </c>
       <c r="G202" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.3">
@@ -6376,7 +6919,10 @@
         <v>2</v>
       </c>
       <c r="C203" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D203" t="s">
+        <v>347</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>110</v>
@@ -6385,7 +6931,7 @@
         <v>138</v>
       </c>
       <c r="G203" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.3">
@@ -6393,16 +6939,19 @@
         <v>2</v>
       </c>
       <c r="C204" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D204" t="s">
+        <v>347</v>
       </c>
       <c r="E204" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F204">
         <v>138</v>
       </c>
       <c r="G204" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.3">
@@ -6410,16 +6959,19 @@
         <v>1</v>
       </c>
       <c r="C205" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D205" t="s">
+        <v>347</v>
       </c>
       <c r="E205" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F205">
         <v>141</v>
       </c>
       <c r="G205" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.3">
@@ -6427,16 +6979,19 @@
         <v>2</v>
       </c>
       <c r="C206" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D206" t="s">
+        <v>347</v>
       </c>
       <c r="E206" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F206">
         <v>142</v>
       </c>
       <c r="G206" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
@@ -6444,16 +6999,19 @@
         <v>2</v>
       </c>
       <c r="C207" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D207" t="s">
+        <v>347</v>
       </c>
       <c r="E207" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F207">
         <v>142</v>
       </c>
       <c r="G207" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.3">
@@ -6461,16 +7019,19 @@
         <v>1</v>
       </c>
       <c r="C208" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D208" t="s">
+        <v>347</v>
       </c>
       <c r="E208" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F208">
         <v>143</v>
       </c>
       <c r="G208" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.3">
@@ -6478,16 +7039,19 @@
         <v>2</v>
       </c>
       <c r="C209" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D209" t="s">
+        <v>347</v>
       </c>
       <c r="E209" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F209">
         <v>144</v>
       </c>
       <c r="G209" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.3">
@@ -6495,16 +7059,19 @@
         <v>5</v>
       </c>
       <c r="C210" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D210" t="s">
+        <v>347</v>
       </c>
       <c r="E210" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F210">
         <v>144</v>
       </c>
       <c r="G210" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.3">
@@ -6512,16 +7079,19 @@
         <v>1</v>
       </c>
       <c r="C211" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D211" t="s">
+        <v>347</v>
       </c>
       <c r="E211" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F211">
         <v>145</v>
       </c>
       <c r="G211" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.3">
@@ -6529,16 +7099,19 @@
         <v>1</v>
       </c>
       <c r="C212" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D212" t="s">
+        <v>347</v>
       </c>
       <c r="E212" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F212">
         <v>145</v>
       </c>
       <c r="G212" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.3">
@@ -6546,16 +7119,19 @@
         <v>1</v>
       </c>
       <c r="C213" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D213" t="s">
+        <v>347</v>
       </c>
       <c r="E213" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F213">
         <v>145</v>
       </c>
       <c r="G213" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.3">
@@ -6563,16 +7139,19 @@
         <v>1</v>
       </c>
       <c r="C214" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D214" t="s">
+        <v>347</v>
       </c>
       <c r="E214" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F214">
         <v>145</v>
       </c>
       <c r="G214" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">
@@ -6580,16 +7159,19 @@
         <v>1</v>
       </c>
       <c r="C215" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D215" t="s">
+        <v>347</v>
       </c>
       <c r="E215" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F215">
         <v>145</v>
       </c>
       <c r="G215" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.3">
@@ -6597,16 +7179,19 @@
         <v>1</v>
       </c>
       <c r="C216" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D216" t="s">
+        <v>347</v>
       </c>
       <c r="E216" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F216">
         <v>145</v>
       </c>
       <c r="G216" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.3">
@@ -6614,16 +7199,19 @@
         <v>1</v>
       </c>
       <c r="C217" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D217" t="s">
+        <v>347</v>
       </c>
       <c r="E217" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F217">
         <v>145</v>
       </c>
       <c r="G217" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.3">
@@ -6631,16 +7219,19 @@
         <v>1</v>
       </c>
       <c r="C218" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D218" t="s">
+        <v>347</v>
       </c>
       <c r="E218" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F218">
         <v>145</v>
       </c>
       <c r="G218" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.3">
@@ -6648,16 +7239,19 @@
         <v>2</v>
       </c>
       <c r="C219" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D219" t="s">
+        <v>347</v>
       </c>
       <c r="E219" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F219">
         <v>146</v>
       </c>
       <c r="G219" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
@@ -6665,16 +7259,19 @@
         <v>2</v>
       </c>
       <c r="C220" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D220" t="s">
+        <v>347</v>
       </c>
       <c r="E220" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F220">
         <v>146</v>
       </c>
       <c r="G220" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
@@ -6682,16 +7279,19 @@
         <v>2</v>
       </c>
       <c r="C221" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D221" t="s">
+        <v>347</v>
       </c>
       <c r="E221" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F221">
         <v>146</v>
       </c>
       <c r="G221" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.3">
@@ -6699,16 +7299,19 @@
         <v>2</v>
       </c>
       <c r="C222" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D222" t="s">
+        <v>347</v>
       </c>
       <c r="E222" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F222">
         <v>146</v>
       </c>
       <c r="G222" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.3">
@@ -6716,16 +7319,19 @@
         <v>2</v>
       </c>
       <c r="C223" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D223" t="s">
+        <v>347</v>
       </c>
       <c r="E223" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F223">
         <v>146</v>
       </c>
       <c r="G223" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.3">
@@ -6733,16 +7339,19 @@
         <v>2</v>
       </c>
       <c r="C224" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D224" t="s">
+        <v>347</v>
       </c>
       <c r="E224" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F224">
         <v>146</v>
       </c>
       <c r="G224" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.3">
@@ -6750,16 +7359,19 @@
         <v>2</v>
       </c>
       <c r="C225" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D225" t="s">
+        <v>347</v>
       </c>
       <c r="E225" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F225">
         <v>146</v>
       </c>
       <c r="G225" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.3">
@@ -6767,16 +7379,19 @@
         <v>2</v>
       </c>
       <c r="C226" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D226" t="s">
+        <v>347</v>
       </c>
       <c r="E226" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F226">
         <v>146</v>
       </c>
       <c r="G226" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.3">
@@ -6784,16 +7399,19 @@
         <v>2</v>
       </c>
       <c r="C227" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D227" t="s">
+        <v>347</v>
       </c>
       <c r="E227" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F227">
         <v>146</v>
       </c>
       <c r="G227" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.3">
@@ -6801,16 +7419,19 @@
         <v>2</v>
       </c>
       <c r="C228" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D228" t="s">
+        <v>347</v>
       </c>
       <c r="E228" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F228">
         <v>146</v>
       </c>
       <c r="G228" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
@@ -6818,16 +7439,19 @@
         <v>2</v>
       </c>
       <c r="C229" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D229" t="s">
+        <v>347</v>
       </c>
       <c r="E229" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F229">
         <v>147</v>
       </c>
       <c r="G229" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
@@ -6835,16 +7459,19 @@
         <v>2</v>
       </c>
       <c r="C230" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D230" t="s">
+        <v>347</v>
       </c>
       <c r="E230" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F230">
         <v>148</v>
       </c>
       <c r="G230" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.3">
@@ -6852,7 +7479,10 @@
         <v>1</v>
       </c>
       <c r="C231" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D231" t="s">
+        <v>347</v>
       </c>
       <c r="E231" s="1" t="s">
         <v>124</v>
@@ -6861,7 +7491,7 @@
         <v>153</v>
       </c>
       <c r="G231" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.3">
@@ -6869,16 +7499,19 @@
         <v>1</v>
       </c>
       <c r="C232" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D232" t="s">
+        <v>347</v>
       </c>
       <c r="E232" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F232">
         <v>153</v>
       </c>
       <c r="G232" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.3">
@@ -6886,7 +7519,10 @@
         <v>2</v>
       </c>
       <c r="C233" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D233" t="s">
+        <v>347</v>
       </c>
       <c r="E233" s="1" t="s">
         <v>124</v>
@@ -6895,7 +7531,7 @@
         <v>154</v>
       </c>
       <c r="G233" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
@@ -6903,16 +7539,19 @@
         <v>2</v>
       </c>
       <c r="C234" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D234" t="s">
+        <v>347</v>
       </c>
       <c r="E234" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F234">
         <v>154</v>
       </c>
       <c r="G234" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.3">
@@ -6920,16 +7559,19 @@
         <v>2</v>
       </c>
       <c r="C235" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D235" t="s">
+        <v>347</v>
       </c>
       <c r="E235" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F235">
         <v>154</v>
       </c>
       <c r="G235" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.3">
@@ -6937,16 +7579,19 @@
         <v>2</v>
       </c>
       <c r="C236" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D236" t="s">
+        <v>347</v>
       </c>
       <c r="E236" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F236">
         <v>154</v>
       </c>
       <c r="G236" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.3">
@@ -6954,16 +7599,19 @@
         <v>1</v>
       </c>
       <c r="C237" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D237" t="s">
+        <v>347</v>
       </c>
       <c r="E237" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F237">
         <v>155</v>
       </c>
       <c r="G237" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.3">
@@ -6971,7 +7619,10 @@
         <v>2</v>
       </c>
       <c r="C238" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D238" t="s">
+        <v>347</v>
       </c>
       <c r="E238" s="1" t="s">
         <v>79</v>
@@ -6980,7 +7631,7 @@
         <v>156</v>
       </c>
       <c r="G238" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.3">
@@ -6988,7 +7639,10 @@
         <v>2</v>
       </c>
       <c r="C239" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D239" t="s">
+        <v>347</v>
       </c>
       <c r="E239" s="1" t="s">
         <v>79</v>
@@ -6997,7 +7651,7 @@
         <v>156</v>
       </c>
       <c r="G239" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
@@ -7005,19 +7659,19 @@
         <v>2</v>
       </c>
       <c r="C240" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D240" t="s">
-        <v>294</v>
+        <v>348</v>
       </c>
       <c r="E240" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F240">
         <v>156</v>
       </c>
       <c r="G240" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.3">
@@ -7025,19 +7679,19 @@
         <v>2</v>
       </c>
       <c r="C241" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D241" t="s">
-        <v>294</v>
+        <v>348</v>
       </c>
       <c r="E241" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F241">
         <v>156</v>
       </c>
       <c r="G241" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.3">
@@ -7045,16 +7699,19 @@
         <v>1</v>
       </c>
       <c r="C242" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D242" t="s">
+        <v>347</v>
       </c>
       <c r="E242" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F242">
         <v>157</v>
       </c>
       <c r="G242" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
@@ -7062,16 +7719,19 @@
         <v>2</v>
       </c>
       <c r="C243" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D243" t="s">
+        <v>347</v>
       </c>
       <c r="E243" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F243">
         <v>158</v>
       </c>
       <c r="G243" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.3">
@@ -7079,16 +7739,19 @@
         <v>2</v>
       </c>
       <c r="C244" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D244" t="s">
+        <v>347</v>
       </c>
       <c r="E244" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F244">
         <v>158</v>
       </c>
       <c r="G244" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
@@ -7096,16 +7759,19 @@
         <v>1</v>
       </c>
       <c r="C245" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D245" t="s">
+        <v>347</v>
       </c>
       <c r="E245" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F245">
         <v>159</v>
       </c>
       <c r="G245" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
@@ -7113,16 +7779,19 @@
         <v>1</v>
       </c>
       <c r="C246" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D246" t="s">
+        <v>347</v>
       </c>
       <c r="E246" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F246">
         <v>159</v>
       </c>
       <c r="G246" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
@@ -7130,16 +7799,19 @@
         <v>1</v>
       </c>
       <c r="C247" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D247" t="s">
+        <v>347</v>
       </c>
       <c r="E247" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F247">
         <v>159</v>
       </c>
       <c r="G247" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
@@ -7147,16 +7819,19 @@
         <v>2</v>
       </c>
       <c r="C248" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D248" t="s">
+        <v>347</v>
       </c>
       <c r="E248" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F248">
         <v>160</v>
       </c>
       <c r="G248" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
@@ -7164,16 +7839,19 @@
         <v>2</v>
       </c>
       <c r="C249" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D249" t="s">
+        <v>347</v>
       </c>
       <c r="E249" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F249">
         <v>160</v>
       </c>
       <c r="G249" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.3">
@@ -7181,16 +7859,19 @@
         <v>2</v>
       </c>
       <c r="C250" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D250" t="s">
+        <v>347</v>
       </c>
       <c r="E250" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F250">
         <v>160</v>
       </c>
       <c r="G250" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
@@ -7198,16 +7879,19 @@
         <v>2</v>
       </c>
       <c r="C251" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D251" t="s">
+        <v>347</v>
       </c>
       <c r="E251" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F251">
         <v>160</v>
       </c>
       <c r="G251" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.3">
@@ -7215,16 +7899,19 @@
         <v>2</v>
       </c>
       <c r="C252" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D252" t="s">
+        <v>347</v>
       </c>
       <c r="E252" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F252">
         <v>160</v>
       </c>
       <c r="G252" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.3">
@@ -7232,16 +7919,19 @@
         <v>2</v>
       </c>
       <c r="C253" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D253" t="s">
+        <v>347</v>
       </c>
       <c r="E253" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F253">
         <v>160</v>
       </c>
       <c r="G253" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
@@ -7249,16 +7939,19 @@
         <v>2</v>
       </c>
       <c r="C254" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D254" t="s">
+        <v>347</v>
       </c>
       <c r="E254" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F254">
         <v>160</v>
       </c>
       <c r="G254" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.3">
@@ -7266,16 +7959,19 @@
         <v>2</v>
       </c>
       <c r="C255" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D255" t="s">
+        <v>347</v>
       </c>
       <c r="E255" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F255">
         <v>160</v>
       </c>
       <c r="G255" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
@@ -7283,16 +7979,19 @@
         <v>2</v>
       </c>
       <c r="C256" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D256" t="s">
+        <v>347</v>
       </c>
       <c r="E256" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F256">
         <v>160</v>
       </c>
       <c r="G256" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.3">
@@ -7300,16 +7999,19 @@
         <v>2</v>
       </c>
       <c r="C257" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D257" t="s">
+        <v>347</v>
       </c>
       <c r="E257" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F257">
         <v>160</v>
       </c>
       <c r="G257" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.3">
@@ -7317,16 +8019,19 @@
         <v>2</v>
       </c>
       <c r="C258" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D258" t="s">
+        <v>347</v>
       </c>
       <c r="E258" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F258">
         <v>160</v>
       </c>
       <c r="G258" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.3">
@@ -7334,16 +8039,19 @@
         <v>2</v>
       </c>
       <c r="C259" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D259" t="s">
+        <v>347</v>
       </c>
       <c r="E259" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F259">
         <v>160</v>
       </c>
       <c r="G259" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.3">
@@ -7351,16 +8059,19 @@
         <v>2</v>
       </c>
       <c r="C260" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D260" t="s">
+        <v>347</v>
       </c>
       <c r="E260" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F260">
         <v>161</v>
       </c>
       <c r="G260" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.3">
@@ -7368,16 +8079,19 @@
         <v>2</v>
       </c>
       <c r="C261" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D261" t="s">
+        <v>347</v>
       </c>
       <c r="E261" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F261">
         <v>161</v>
       </c>
       <c r="G261" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
@@ -7385,16 +8099,19 @@
         <v>2</v>
       </c>
       <c r="C262" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D262" t="s">
+        <v>347</v>
       </c>
       <c r="E262" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F262">
         <v>161</v>
       </c>
       <c r="G262" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.3">
@@ -7402,16 +8119,19 @@
         <v>2</v>
       </c>
       <c r="C263" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D263" t="s">
+        <v>347</v>
       </c>
       <c r="E263" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F263">
         <v>161</v>
       </c>
       <c r="G263" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.3">
@@ -7419,16 +8139,19 @@
         <v>2</v>
       </c>
       <c r="C264" t="s">
-        <v>316</v>
+        <v>312</v>
+      </c>
+      <c r="D264" t="s">
+        <v>347</v>
       </c>
       <c r="E264" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F264">
         <v>162</v>
       </c>
       <c r="G264" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.3">
@@ -7436,16 +8159,19 @@
         <v>2</v>
       </c>
       <c r="C265" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="D265" t="s">
+        <v>347</v>
       </c>
       <c r="E265" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F265">
         <v>162</v>
       </c>
       <c r="G265" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>